<commit_message>
Priority, Team Roles, Tasks and Sprint 1 defined, updated
</commit_message>
<xml_diff>
--- a/System Development/Product backlog v2.xlsx
+++ b/System Development/Product backlog v2.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Details" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="3" r:id="rId3"/>
+    <sheet name="Team Roles" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="150">
   <si>
     <t>ID</t>
   </si>
@@ -77,18 +79,9 @@
     <t>I can remove myself from searches</t>
   </si>
   <si>
-    <t>Search</t>
-  </si>
-  <si>
     <t>I can send a Connection request</t>
   </si>
   <si>
-    <t>Accept connection request</t>
-  </si>
-  <si>
-    <t>Remove/decline</t>
-  </si>
-  <si>
     <t>Be able to remove/decline connection request</t>
   </si>
   <si>
@@ -107,9 +100,6 @@
     <t>Be able to report another user</t>
   </si>
   <si>
-    <t>I can remove spammer and anoying people</t>
-  </si>
-  <si>
     <t>Send message</t>
   </si>
   <si>
@@ -119,12 +109,6 @@
     <t>Be able to search the search for other people with certain passions</t>
   </si>
   <si>
-    <t>Narrow serach</t>
-  </si>
-  <si>
-    <t>Be able to narrow a seach by criteria</t>
-  </si>
-  <si>
     <t>I can find certain people(closer, far away..)</t>
   </si>
   <si>
@@ -197,15 +181,6 @@
     <t>Administrator</t>
   </si>
   <si>
-    <t>Buy help</t>
-  </si>
-  <si>
-    <t>Be able to ask for paid help</t>
-  </si>
-  <si>
-    <t>I can get help immediately</t>
-  </si>
-  <si>
     <t>Block users from app</t>
   </si>
   <si>
@@ -275,9 +250,6 @@
     <t>Remove users rights</t>
   </si>
   <si>
-    <t>Be able to derank and administrator to become a user.</t>
-  </si>
-  <si>
     <t>I can fire people.</t>
   </si>
   <si>
@@ -372,6 +344,129 @@
   </si>
   <si>
     <t>In the store the user can purchase online help. Purchasing the package will allow the user to message a 24/7 help service.</t>
+  </si>
+  <si>
+    <t>Narrow search</t>
+  </si>
+  <si>
+    <t>Be able to narrow a search by criteria</t>
+  </si>
+  <si>
+    <t>Remove/decline request</t>
+  </si>
+  <si>
+    <t>I can remove spammer and annoying people</t>
+  </si>
+  <si>
+    <t>Book assistance</t>
+  </si>
+  <si>
+    <t>Book an advisor</t>
+  </si>
+  <si>
+    <t>I can book an advisor and ask for help</t>
+  </si>
+  <si>
+    <t>Be able to drank an administrator to become a user.</t>
+  </si>
+  <si>
+    <t>Story points</t>
+  </si>
+  <si>
+    <t>Search and show</t>
+  </si>
+  <si>
+    <t>Accept &amp; Matching</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Start Search</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>story</t>
+  </si>
+  <si>
+    <t>tasks</t>
+  </si>
+  <si>
+    <t>create database, register interface, connections, querries</t>
+  </si>
+  <si>
+    <t>login interface, connections, querries</t>
+  </si>
+  <si>
+    <t>search algorythm, retrieve info order, compare data,</t>
+  </si>
+  <si>
+    <t>Scrum Master</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Programmer</t>
+  </si>
+  <si>
+    <t>Ionut</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>2nd programmer</t>
+  </si>
+  <si>
+    <t>Report Writing, Candidate Class Diagram - Richard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo - Design Class Diagram, Technology Report, </t>
+  </si>
+  <si>
+    <t>Stand up meeting agreement</t>
+  </si>
+  <si>
+    <t>when not at school</t>
+  </si>
+  <si>
+    <t>when at school</t>
+  </si>
+  <si>
+    <t>summarizing previous results</t>
+  </si>
+  <si>
+    <t>deciding on following steps</t>
+  </si>
+  <si>
+    <t>checking milestones</t>
+  </si>
+  <si>
+    <t>Development Environment</t>
+  </si>
+  <si>
+    <t>Have all software on all the laptops</t>
+  </si>
+  <si>
+    <t>We use Visual Studio for coding in C#</t>
+  </si>
+  <si>
+    <t>Test phone is a Windows Phone running on Windows 8</t>
   </si>
 </sst>
 </file>
@@ -446,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -458,9 +553,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -476,7 +572,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -762,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,9 +871,10 @@
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -797,12 +894,15 @@
         <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -818,12 +918,17 @@
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="1"/>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -839,12 +944,17 @@
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -862,8 +972,9 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -881,431 +992,489 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>6</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="2">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>30</v>
+        <v>112</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="F13" s="2">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2">
+        <v>10</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F14" s="2">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2">
+        <v>4</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2">
+        <v>12</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1318,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,10 +1503,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -1345,10 +1514,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1356,10 +1525,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1367,10 +1536,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1378,10 +1547,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1389,7 +1558,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C6" s="7"/>
     </row>
@@ -1398,7 +1567,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C7" s="7"/>
     </row>
@@ -1407,7 +1576,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C8" s="7"/>
     </row>
@@ -1416,7 +1585,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C9" s="7"/>
     </row>
@@ -1425,7 +1594,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C10" s="7"/>
     </row>
@@ -1434,7 +1603,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C11" s="7"/>
     </row>
@@ -1443,10 +1612,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1454,10 +1623,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1465,7 +1634,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C14" s="7"/>
     </row>
@@ -1474,10 +1643,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -1485,10 +1654,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1496,10 +1665,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1507,10 +1676,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1518,10 +1687,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1529,10 +1698,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1588,4 +1757,192 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="B9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sprint Backlog and Report Update
</commit_message>
<xml_diff>
--- a/System Development/Product backlog v2.xlsx
+++ b/System Development/Product backlog v2.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="199">
   <si>
     <t>ID</t>
   </si>
@@ -595,6 +595,36 @@
   </si>
   <si>
     <t>Connect list with PP</t>
+  </si>
+  <si>
+    <t>work time</t>
+  </si>
+  <si>
+    <t>4 hour/day</t>
+  </si>
+  <si>
+    <t>5 days / week</t>
+  </si>
+  <si>
+    <t>sprint 1</t>
+  </si>
+  <si>
+    <t>sprint 2</t>
+  </si>
+  <si>
+    <t>sprint 3</t>
+  </si>
+  <si>
+    <t>sprint 4</t>
+  </si>
+  <si>
+    <t>20 hours / week</t>
+  </si>
+  <si>
+    <t>80 hours total</t>
+  </si>
+  <si>
+    <t>1 SP = 1,194 hour</t>
   </si>
 </sst>
 </file>
@@ -721,15 +751,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1013,7 +1043,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="H12" sqref="H11:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1254,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1950,7 +1980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -2107,10 +2137,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,27 +2148,37 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E1" s="10" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E1" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>168</v>
       </c>
       <c r="D2" t="s">
@@ -2165,152 +2205,591 @@
       <c r="K2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="N2">
+        <v>67</v>
+      </c>
+      <c r="O2" t="s">
+        <v>190</v>
+      </c>
+      <c r="P2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>150</v>
       </c>
       <c r="D3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="15" t="s">
+      <c r="E3">
+        <v>2.5</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="14" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="15" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>197</v>
+      </c>
+      <c r="P4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="14" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="15" t="s">
+      <c r="E5">
+        <v>3.5</v>
+      </c>
+      <c r="F5">
+        <v>3.5</v>
+      </c>
+      <c r="G5">
+        <v>2.5</v>
+      </c>
+      <c r="H5">
+        <v>2.5</v>
+      </c>
+      <c r="I5">
+        <v>2.5</v>
+      </c>
+      <c r="J5">
+        <v>2.5</v>
+      </c>
+      <c r="K5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="14" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="12" t="s">
+      <c r="E6">
+        <v>2.5</v>
+      </c>
+      <c r="F6">
+        <v>2.5</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>192</v>
+      </c>
+      <c r="N6">
+        <v>13</v>
+      </c>
+      <c r="O6">
+        <f>13*1.194</f>
+        <v>15.521999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>151</v>
       </c>
       <c r="D7" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="15" t="s">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>193</v>
+      </c>
+      <c r="N7">
+        <v>19</v>
+      </c>
+      <c r="O7">
+        <f>19*1.194</f>
+        <v>22.686</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="14" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="15" t="s">
+      <c r="E8">
+        <v>2.5</v>
+      </c>
+      <c r="F8">
+        <v>2.5</v>
+      </c>
+      <c r="G8">
+        <v>2.5</v>
+      </c>
+      <c r="H8">
+        <v>2.5</v>
+      </c>
+      <c r="I8">
+        <v>2.5</v>
+      </c>
+      <c r="J8">
+        <v>2.5</v>
+      </c>
+      <c r="K8">
+        <v>2.5</v>
+      </c>
+      <c r="M8" t="s">
+        <v>194</v>
+      </c>
+      <c r="N8">
+        <v>9</v>
+      </c>
+      <c r="O8">
+        <f>9*1.194</f>
+        <v>10.745999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="14" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="15"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="E9">
+        <v>2.5</v>
+      </c>
+      <c r="F9">
+        <v>2.5</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>195</v>
+      </c>
+      <c r="N9">
+        <v>26</v>
+      </c>
+      <c r="O9">
+        <f>26*1.194</f>
+        <v>31.043999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
         <v>2</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>182</v>
       </c>
       <c r="D11" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="11" t="s">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>150</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <f>N11*1.194</f>
+        <v>2.3879999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="11" t="s">
+      <c r="E12">
+        <v>12</v>
+      </c>
+      <c r="M12" t="s">
+        <v>179</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12:O28" si="0">N12*1.194</f>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="10" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="11" t="s">
+      <c r="E13">
+        <v>2.5</v>
+      </c>
+      <c r="M13" t="s">
+        <v>180</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>3.5819999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="10" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="16" t="s">
+      <c r="E14">
+        <v>2.5</v>
+      </c>
+      <c r="M14" t="s">
+        <v>149</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>2.3879999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="11" t="s">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>151</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="10" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="11" t="s">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>180</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>2.3879999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="16" t="s">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>149</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>2.3879999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="11" t="s">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="10" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="11" t="s">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>182</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="0"/>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="10" t="s">
         <v>188</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="M20" t="s">
+        <v>183</v>
+      </c>
+      <c r="N20">
+        <v>10</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>11.94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>184</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="0"/>
+        <v>2.3879999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>185</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>2.3879999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>159</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>186</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>162</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="0"/>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>163</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>187</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>1.194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>188</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>1.194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>